<commit_message>
Databases module 10 # add triggers and validations on DB level and additional calculations for SELECT queries
</commit_message>
<xml_diff>
--- a/calculations/calculations.xlsx
+++ b/calculations/calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yevgeniy_Protas\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB952BB0-FF73-4A38-BF3B-E9508EEECD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815DB839-A53E-4FE8-8F2C-5B7F33F7CA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE25C8A8-E171-4690-8A6A-7FA5B543C96A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="23">
   <si>
     <t>Таблица</t>
   </si>
@@ -85,6 +85,24 @@
   </si>
   <si>
     <t>exam_result</t>
+  </si>
+  <si>
+    <t>SELECT</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Условие</t>
+  </si>
+  <si>
+    <t>Find user by name (exact match)</t>
+  </si>
+  <si>
+    <t>Find user by surname (partial match)</t>
+  </si>
+  <si>
+    <t>Find user by phone number (partial match)</t>
   </si>
 </sst>
 </file>
@@ -163,7 +181,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -216,6 +234,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -224,7 +292,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -238,6 +306,19 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -556,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD95307C-5D33-4C89-9A1C-59EFABA30DDE}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,9 +651,10 @@
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,8 +673,11 @@
       <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -608,11 +693,12 @@
       <c r="E2" s="2">
         <v>6</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="6">
         <v>2166</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -628,11 +714,12 @@
       <c r="E3" s="2">
         <v>43</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -648,11 +735,12 @@
       <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="6">
         <v>2181</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -668,11 +756,12 @@
       <c r="E5" s="2">
         <v>10</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="6">
         <v>3477</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -688,71 +777,81 @@
       <c r="E6" s="2">
         <v>0</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="6">
         <v>1905</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1000</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2">
+        <v>100000</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="3">
-        <v>1000</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="E7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="6">
+        <v>669</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2">
+        <v>200</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="6">
         <v>5</v>
       </c>
-      <c r="E8" s="3">
-        <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="F8" s="3">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1000</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="3">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="F9" s="3">
+      <c r="G8" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2">
+        <v>200</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="6">
+        <v>4</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -763,16 +862,17 @@
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10" s="3">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="F10" s="3">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7">
+        <v>31</v>
+      </c>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -783,76 +883,80 @@
         <v>4</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E11" s="3">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="7">
+        <v>38</v>
+      </c>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="F12" s="7">
+        <v>18</v>
+      </c>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="F13" s="7">
+        <v>28</v>
+      </c>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="F14" s="7">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="4">
-        <v>1000000</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0</v>
-      </c>
-      <c r="F12" s="4">
-        <v>15951</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="4">
-        <v>1000000</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="4">
-        <v>59</v>
-      </c>
-      <c r="F13" s="4">
-        <v>26560</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="4">
-        <v>1000000</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="4">
-        <v>448</v>
-      </c>
-      <c r="F14" s="4">
-        <v>497840</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -863,16 +967,17 @@
         <v>4</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E15" s="4">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="F15" s="4">
-        <v>20819</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F15" s="8">
+        <v>15951</v>
+      </c>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -883,17 +988,82 @@
         <v>4</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="4">
+        <v>59</v>
+      </c>
+      <c r="F16" s="8">
+        <v>26560</v>
+      </c>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="4">
+        <v>448</v>
+      </c>
+      <c r="F17" s="8">
+        <v>497840</v>
+      </c>
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="F18" s="8">
+        <v>20819</v>
+      </c>
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E19" s="4">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F19" s="8">
         <v>23938</v>
       </c>
+      <c r="G19" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>